<commit_message>
extended data fig 2
</commit_message>
<xml_diff>
--- a/supplementary/data2/randomized.xlsx
+++ b/supplementary/data2/randomized.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="simulation" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="fit" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="description" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="simulation" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="fit" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="description" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,31 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Nc</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Fc</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>seed</t>
         </is>
       </c>
@@ -518,9 +543,24 @@
         <v>150</v>
       </c>
       <c r="J2" t="n">
-        <v>2.408927440643311</v>
+        <v>2.408927484817753</v>
       </c>
       <c r="K2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L2" t="n">
+        <v>500</v>
+      </c>
+      <c r="M2" t="n">
+        <v>5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>500</v>
+      </c>
+      <c r="O2" t="n">
+        <v>14</v>
+      </c>
+      <c r="P2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -555,9 +595,24 @@
         <v>150</v>
       </c>
       <c r="J3" t="n">
-        <v>5.276147365570068</v>
+        <v>5.276147516638866</v>
       </c>
       <c r="K3" t="n">
+        <v>5</v>
+      </c>
+      <c r="L3" t="n">
+        <v>500</v>
+      </c>
+      <c r="M3" t="n">
+        <v>5</v>
+      </c>
+      <c r="N3" t="n">
+        <v>500</v>
+      </c>
+      <c r="O3" t="n">
+        <v>14</v>
+      </c>
+      <c r="P3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -592,9 +647,24 @@
         <v>150</v>
       </c>
       <c r="J4" t="n">
-        <v>2.271743059158325</v>
+        <v>2.271743131132066</v>
       </c>
       <c r="K4" t="n">
+        <v>5</v>
+      </c>
+      <c r="L4" t="n">
+        <v>500</v>
+      </c>
+      <c r="M4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N4" t="n">
+        <v>500</v>
+      </c>
+      <c r="O4" t="n">
+        <v>14</v>
+      </c>
+      <c r="P4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -629,9 +699,24 @@
         <v>150</v>
       </c>
       <c r="J5" t="n">
-        <v>4.23241138458252</v>
+        <v>4.232411760370248</v>
       </c>
       <c r="K5" t="n">
+        <v>5</v>
+      </c>
+      <c r="L5" t="n">
+        <v>500</v>
+      </c>
+      <c r="M5" t="n">
+        <v>5</v>
+      </c>
+      <c r="N5" t="n">
+        <v>500</v>
+      </c>
+      <c r="O5" t="n">
+        <v>14</v>
+      </c>
+      <c r="P5" t="n">
         <v>3</v>
       </c>
     </row>
@@ -666,9 +751,24 @@
         <v>150</v>
       </c>
       <c r="J6" t="n">
-        <v>4.246438026428223</v>
+        <v>4.246437958756789</v>
       </c>
       <c r="K6" t="n">
+        <v>5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>500</v>
+      </c>
+      <c r="M6" t="n">
+        <v>5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>500</v>
+      </c>
+      <c r="O6" t="n">
+        <v>14</v>
+      </c>
+      <c r="P6" t="n">
         <v>4</v>
       </c>
     </row>
@@ -703,9 +803,24 @@
         <v>150</v>
       </c>
       <c r="J7" t="n">
-        <v>2.775936365127563</v>
+        <v>2.77593638767674</v>
       </c>
       <c r="K7" t="n">
+        <v>5</v>
+      </c>
+      <c r="L7" t="n">
+        <v>500</v>
+      </c>
+      <c r="M7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" t="n">
+        <v>500</v>
+      </c>
+      <c r="O7" t="n">
+        <v>14</v>
+      </c>
+      <c r="P7" t="n">
         <v>5</v>
       </c>
     </row>
@@ -740,9 +855,24 @@
         <v>150</v>
       </c>
       <c r="J8" t="n">
-        <v>2.480589866638184</v>
+        <v>2.480589919612951</v>
       </c>
       <c r="K8" t="n">
+        <v>5</v>
+      </c>
+      <c r="L8" t="n">
+        <v>500</v>
+      </c>
+      <c r="M8" t="n">
+        <v>5</v>
+      </c>
+      <c r="N8" t="n">
+        <v>500</v>
+      </c>
+      <c r="O8" t="n">
+        <v>14</v>
+      </c>
+      <c r="P8" t="n">
         <v>6</v>
       </c>
     </row>
@@ -777,9 +907,24 @@
         <v>150</v>
       </c>
       <c r="J9" t="n">
-        <v>3.71852707862854</v>
+        <v>3.718527160375618</v>
       </c>
       <c r="K9" t="n">
+        <v>5</v>
+      </c>
+      <c r="L9" t="n">
+        <v>500</v>
+      </c>
+      <c r="M9" t="n">
+        <v>5</v>
+      </c>
+      <c r="N9" t="n">
+        <v>500</v>
+      </c>
+      <c r="O9" t="n">
+        <v>14</v>
+      </c>
+      <c r="P9" t="n">
         <v>7</v>
       </c>
     </row>
@@ -814,9 +959,24 @@
         <v>150</v>
       </c>
       <c r="J10" t="n">
-        <v>4.316863059997559</v>
+        <v>4.316863430182595</v>
       </c>
       <c r="K10" t="n">
+        <v>5</v>
+      </c>
+      <c r="L10" t="n">
+        <v>500</v>
+      </c>
+      <c r="M10" t="n">
+        <v>5</v>
+      </c>
+      <c r="N10" t="n">
+        <v>500</v>
+      </c>
+      <c r="O10" t="n">
+        <v>14</v>
+      </c>
+      <c r="P10" t="n">
         <v>8</v>
       </c>
     </row>
@@ -851,9 +1011,24 @@
         <v>150</v>
       </c>
       <c r="J11" t="n">
-        <v>3.177313089370728</v>
+        <v>3.177313224213249</v>
       </c>
       <c r="K11" t="n">
+        <v>5</v>
+      </c>
+      <c r="L11" t="n">
+        <v>500</v>
+      </c>
+      <c r="M11" t="n">
+        <v>5</v>
+      </c>
+      <c r="N11" t="n">
+        <v>500</v>
+      </c>
+      <c r="O11" t="n">
+        <v>14</v>
+      </c>
+      <c r="P11" t="n">
         <v>9</v>
       </c>
     </row>
@@ -888,9 +1063,24 @@
         <v>150</v>
       </c>
       <c r="J12" t="n">
-        <v>2.888209581375122</v>
+        <v>2.88820952399692</v>
       </c>
       <c r="K12" t="n">
+        <v>5</v>
+      </c>
+      <c r="L12" t="n">
+        <v>500</v>
+      </c>
+      <c r="M12" t="n">
+        <v>5</v>
+      </c>
+      <c r="N12" t="n">
+        <v>500</v>
+      </c>
+      <c r="O12" t="n">
+        <v>14</v>
+      </c>
+      <c r="P12" t="n">
         <v>10</v>
       </c>
     </row>
@@ -925,9 +1115,24 @@
         <v>150</v>
       </c>
       <c r="J13" t="n">
-        <v>3.210572004318237</v>
+        <v>3.210571946228199</v>
       </c>
       <c r="K13" t="n">
+        <v>5</v>
+      </c>
+      <c r="L13" t="n">
+        <v>500</v>
+      </c>
+      <c r="M13" t="n">
+        <v>5</v>
+      </c>
+      <c r="N13" t="n">
+        <v>500</v>
+      </c>
+      <c r="O13" t="n">
+        <v>14</v>
+      </c>
+      <c r="P13" t="n">
         <v>11</v>
       </c>
     </row>
@@ -962,9 +1167,24 @@
         <v>150</v>
       </c>
       <c r="J14" t="n">
-        <v>3.142275333404541</v>
+        <v>3.142275445563244</v>
       </c>
       <c r="K14" t="n">
+        <v>5</v>
+      </c>
+      <c r="L14" t="n">
+        <v>500</v>
+      </c>
+      <c r="M14" t="n">
+        <v>5</v>
+      </c>
+      <c r="N14" t="n">
+        <v>500</v>
+      </c>
+      <c r="O14" t="n">
+        <v>14</v>
+      </c>
+      <c r="P14" t="n">
         <v>12</v>
       </c>
     </row>
@@ -999,9 +1219,24 @@
         <v>150</v>
       </c>
       <c r="J15" t="n">
-        <v>4.087015151977539</v>
+        <v>4.087015034999207</v>
       </c>
       <c r="K15" t="n">
+        <v>5</v>
+      </c>
+      <c r="L15" t="n">
+        <v>500</v>
+      </c>
+      <c r="M15" t="n">
+        <v>5</v>
+      </c>
+      <c r="N15" t="n">
+        <v>500</v>
+      </c>
+      <c r="O15" t="n">
+        <v>14</v>
+      </c>
+      <c r="P15" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1036,9 +1271,24 @@
         <v>150</v>
       </c>
       <c r="J16" t="n">
-        <v>5.713561058044434</v>
+        <v>5.713560674905024</v>
       </c>
       <c r="K16" t="n">
+        <v>5</v>
+      </c>
+      <c r="L16" t="n">
+        <v>500</v>
+      </c>
+      <c r="M16" t="n">
+        <v>5</v>
+      </c>
+      <c r="N16" t="n">
+        <v>500</v>
+      </c>
+      <c r="O16" t="n">
+        <v>14</v>
+      </c>
+      <c r="P16" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1073,9 +1323,24 @@
         <v>150</v>
       </c>
       <c r="J17" t="n">
-        <v>2.261444330215454</v>
+        <v>2.261444487873829</v>
       </c>
       <c r="K17" t="n">
+        <v>5</v>
+      </c>
+      <c r="L17" t="n">
+        <v>500</v>
+      </c>
+      <c r="M17" t="n">
+        <v>5</v>
+      </c>
+      <c r="N17" t="n">
+        <v>500</v>
+      </c>
+      <c r="O17" t="n">
+        <v>14</v>
+      </c>
+      <c r="P17" t="n">
         <v>15</v>
       </c>
     </row>
@@ -1110,9 +1375,24 @@
         <v>150</v>
       </c>
       <c r="J18" t="n">
-        <v>3.545289993286133</v>
+        <v>3.545290009011557</v>
       </c>
       <c r="K18" t="n">
+        <v>5</v>
+      </c>
+      <c r="L18" t="n">
+        <v>500</v>
+      </c>
+      <c r="M18" t="n">
+        <v>5</v>
+      </c>
+      <c r="N18" t="n">
+        <v>500</v>
+      </c>
+      <c r="O18" t="n">
+        <v>14</v>
+      </c>
+      <c r="P18" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1127,7 +1407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:AB18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1203,55 +1483,70 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
+          <t>Keq_mean</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Keq_ll</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Keq_ul</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>MCC</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Recall</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Precision</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>TN</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>FP</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>FN</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>TP</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>z_median</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>z_ll</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>z_ul</t>
-        </is>
-      </c>
       <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)_median</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)_ll</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)_ul</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>seed</t>
         </is>
@@ -1264,75 +1559,84 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.438702344894409</v>
+        <v>2.450336179885969</v>
       </c>
       <c r="C2" t="n">
-        <v>17.10677719116211</v>
+        <v>17.16527117559449</v>
       </c>
       <c r="D2" t="n">
-        <v>17.10677719116211</v>
+        <v>17.11842457348393</v>
       </c>
       <c r="E2" t="n">
-        <v>17.10677719116211</v>
+        <v>17.21309306380971</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1396523714065552</v>
+        <v>0.1681755578235359</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1396523714065552</v>
+        <v>0.1535863291072242</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1396523714065552</v>
+        <v>0.182523608550857</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4887973368167877</v>
+        <v>0.4918823660806131</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4887973368167877</v>
+        <v>0.4739967091488309</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4887973368167877</v>
+        <v>0.5101703184095499</v>
       </c>
       <c r="L2" t="n">
-        <v>0.3716797530651093</v>
+        <v>0.3954936010733465</v>
       </c>
       <c r="M2" t="n">
-        <v>0.3716797530651093</v>
+        <v>0.3745493803287874</v>
       </c>
       <c r="N2" t="n">
-        <v>0.3716797530651093</v>
+        <v>0.4176100891635587</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9134347535906021</v>
+        <v>0.2023959289118014</v>
       </c>
       <c r="P2" t="n">
-        <v>0.930835734870317</v>
+        <v>0.1814553993564418</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.9202279202279202</v>
+        <v>0.2232769172971851</v>
       </c>
       <c r="R2" t="n">
-        <v>2125</v>
+        <v>0.9264201029975682</v>
       </c>
       <c r="S2" t="n">
-        <v>28</v>
+        <v>0.9534313725490197</v>
       </c>
       <c r="T2" t="n">
-        <v>24</v>
+        <v>0.9239904988123515</v>
       </c>
       <c r="U2" t="n">
-        <v>323</v>
+        <v>2060</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9750985503196716</v>
+        <v>32</v>
       </c>
       <c r="W2" t="n">
-        <v>0.9404993057250977</v>
+        <v>19</v>
       </c>
       <c r="X2" t="n">
-        <v>0.9858063459396362</v>
+        <v>389</v>
       </c>
       <c r="Y2" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.9163600000000001</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.986</v>
+      </c>
+      <c r="AB2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1343,75 +1647,84 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.431694984436035</v>
+        <v>5.481635293610579</v>
       </c>
       <c r="C3" t="n">
-        <v>3.570416688919067</v>
+        <v>3.566288122454535</v>
       </c>
       <c r="D3" t="n">
-        <v>3.570416688919067</v>
+        <v>3.556111233910164</v>
       </c>
       <c r="E3" t="n">
-        <v>3.570416688919067</v>
+        <v>3.575927473450315</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1421861797571182</v>
+        <v>0.1320079901725598</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1421861797571182</v>
+        <v>0.1163468435004809</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1421861797571182</v>
+        <v>0.1462326187511007</v>
       </c>
       <c r="I3" t="n">
-        <v>0.4912124872207642</v>
+        <v>0.4888621493178085</v>
       </c>
       <c r="J3" t="n">
-        <v>0.4912124872207642</v>
+        <v>0.4721525900008338</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4912124872207642</v>
+        <v>0.50866117650181</v>
       </c>
       <c r="L3" t="n">
-        <v>0.3815518915653229</v>
+        <v>0.3777703335944265</v>
       </c>
       <c r="M3" t="n">
-        <v>0.3815518915653229</v>
+        <v>0.3584790276930416</v>
       </c>
       <c r="N3" t="n">
-        <v>0.3815518915653229</v>
+        <v>0.4006017276722568</v>
       </c>
       <c r="O3" t="n">
-        <v>0.952886292636252</v>
+        <v>0.1512817623472566</v>
       </c>
       <c r="P3" t="n">
-        <v>0.9717514124293786</v>
+        <v>0.1316658010941941</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.9476584022038568</v>
+        <v>0.1712792425886149</v>
       </c>
       <c r="R3" t="n">
-        <v>2127</v>
+        <v>0.9645890834486046</v>
       </c>
       <c r="S3" t="n">
-        <v>19</v>
+        <v>0.9822485207100592</v>
       </c>
       <c r="T3" t="n">
-        <v>10</v>
+        <v>0.9567723342939481</v>
       </c>
       <c r="U3" t="n">
-        <v>344</v>
+        <v>2147</v>
       </c>
       <c r="V3" t="n">
-        <v>0.9759342670440674</v>
+        <v>15</v>
       </c>
       <c r="W3" t="n">
-        <v>0.9404127597808838</v>
+        <v>6</v>
       </c>
       <c r="X3" t="n">
-        <v>0.9881094098091125</v>
+        <v>332</v>
       </c>
       <c r="Y3" t="n">
+        <v>0.972</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.9073599999999999</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="AB3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1422,75 +1735,84 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.313198328018188</v>
+        <v>2.315013238432216</v>
       </c>
       <c r="C4" t="n">
-        <v>19.34237289428711</v>
+        <v>19.3922756019917</v>
       </c>
       <c r="D4" t="n">
-        <v>19.34237289428711</v>
+        <v>19.33912647947308</v>
       </c>
       <c r="E4" t="n">
-        <v>19.34237289428711</v>
+        <v>19.44336897403454</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1881111413240433</v>
+        <v>0.1806256028942435</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1881111413240433</v>
+        <v>0.1658899786984948</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1881111413240433</v>
+        <v>0.1954344789468285</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6234095096588135</v>
+        <v>0.6357641268868417</v>
       </c>
       <c r="J4" t="n">
-        <v>0.6234095096588135</v>
+        <v>0.6156477734409387</v>
       </c>
       <c r="K4" t="n">
-        <v>0.6234095096588135</v>
+        <v>0.6573685962339372</v>
       </c>
       <c r="L4" t="n">
-        <v>0.3831014335155487</v>
+        <v>0.3641918289843784</v>
       </c>
       <c r="M4" t="n">
-        <v>0.3831014335155487</v>
+        <v>0.3444265066326494</v>
       </c>
       <c r="N4" t="n">
-        <v>0.3831014335155487</v>
+        <v>0.3871126474843582</v>
       </c>
       <c r="O4" t="n">
-        <v>0.9105544908475063</v>
+        <v>0.2208806236964063</v>
       </c>
       <c r="P4" t="n">
-        <v>0.9305263157894736</v>
+        <v>0.1988826160007507</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.9246861924686193</v>
+        <v>0.2429068625594686</v>
       </c>
       <c r="R4" t="n">
-        <v>1989</v>
+        <v>0.90819662727734</v>
       </c>
       <c r="S4" t="n">
+        <v>0.9297052154195011</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.9192825112107623</v>
+      </c>
+      <c r="U4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="V4" t="n">
         <v>36</v>
       </c>
-      <c r="T4" t="n">
-        <v>33</v>
-      </c>
-      <c r="U4" t="n">
-        <v>442</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0.9759545922279358</v>
-      </c>
       <c r="W4" t="n">
-        <v>0.933514416217804</v>
+        <v>31</v>
       </c>
       <c r="X4" t="n">
-        <v>0.9875326752662659</v>
+        <v>410</v>
       </c>
       <c r="Y4" t="n">
+        <v>0.971</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0.985</v>
+      </c>
+      <c r="AB4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1501,75 +1823,84 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.361331939697266</v>
+        <v>4.313936268572636</v>
       </c>
       <c r="C5" t="n">
-        <v>5.56596565246582</v>
+        <v>5.569011179321521</v>
       </c>
       <c r="D5" t="n">
-        <v>5.56596565246582</v>
+        <v>5.553981809194724</v>
       </c>
       <c r="E5" t="n">
-        <v>5.56596565246582</v>
+        <v>5.583577874255999</v>
       </c>
       <c r="F5" t="n">
-        <v>0.08884377777576447</v>
+        <v>0.09452236784607207</v>
       </c>
       <c r="G5" t="n">
-        <v>0.08884377777576447</v>
+        <v>0.08455107744832235</v>
       </c>
       <c r="H5" t="n">
-        <v>0.08884377777576447</v>
+        <v>0.1053655473805682</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6178345680236816</v>
+        <v>0.6371056465631558</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6178345680236816</v>
+        <v>0.6166066211244072</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6178345680236816</v>
+        <v>0.6546946844822619</v>
       </c>
       <c r="L5" t="n">
-        <v>0.2343354076147079</v>
+        <v>0.25506299532828</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2343354076147079</v>
+        <v>0.2375422694298888</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2343354076147079</v>
+        <v>0.2721699984757414</v>
       </c>
       <c r="O5" t="n">
-        <v>0.9196077719375807</v>
+        <v>0.1041981755927499</v>
       </c>
       <c r="P5" t="n">
-        <v>0.9033613445378151</v>
+        <v>0.09236023491029278</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.9513274336283186</v>
+        <v>0.1177750277380042</v>
       </c>
       <c r="R5" t="n">
-        <v>2251</v>
+        <v>0.9349982645915699</v>
       </c>
       <c r="S5" t="n">
-        <v>11</v>
+        <v>0.9471544715447154</v>
       </c>
       <c r="T5" t="n">
-        <v>23</v>
+        <v>0.9357429718875502</v>
       </c>
       <c r="U5" t="n">
-        <v>215</v>
+        <v>2238</v>
       </c>
       <c r="V5" t="n">
-        <v>0.9798104763031006</v>
+        <v>16</v>
       </c>
       <c r="W5" t="n">
-        <v>0.9126093983650208</v>
+        <v>13</v>
       </c>
       <c r="X5" t="n">
-        <v>0.9898970127105713</v>
+        <v>233</v>
       </c>
       <c r="Y5" t="n">
+        <v>0.9735</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.9104</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0.988</v>
+      </c>
+      <c r="AB5" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1580,75 +1911,84 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.190643787384033</v>
+        <v>4.224484032453902</v>
       </c>
       <c r="C6" t="n">
-        <v>5.501767635345459</v>
+        <v>5.510981805879009</v>
       </c>
       <c r="D6" t="n">
-        <v>5.501767635345459</v>
+        <v>5.496036903002576</v>
       </c>
       <c r="E6" t="n">
-        <v>5.501767635345459</v>
+        <v>5.525636382040267</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01392489671707153</v>
+        <v>0.01657650639560423</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01392489671707153</v>
+        <v>0.0120207823373627</v>
       </c>
       <c r="H6" t="n">
-        <v>0.01392489671707153</v>
+        <v>0.02309030589589533</v>
       </c>
       <c r="I6" t="n">
-        <v>0.06444264948368073</v>
+        <v>0.07156419810671874</v>
       </c>
       <c r="J6" t="n">
-        <v>0.06444264948368073</v>
+        <v>0.06457248704463925</v>
       </c>
       <c r="K6" t="n">
-        <v>0.06444264948368073</v>
+        <v>0.07854689277434543</v>
       </c>
       <c r="L6" t="n">
-        <v>0.3973357379436493</v>
+        <v>0.4320396496649736</v>
       </c>
       <c r="M6" t="n">
-        <v>0.3973357379436493</v>
+        <v>0.357821782022664</v>
       </c>
       <c r="N6" t="n">
-        <v>0.3973357379436493</v>
+        <v>0.5155956999809113</v>
       </c>
       <c r="O6" t="n">
-        <v>0.931303987393397</v>
+        <v>0.01705742658344456</v>
       </c>
       <c r="P6" t="n">
-        <v>0.9714285714285714</v>
+        <v>0.01216704080033983</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.8947368421052632</v>
+        <v>0.02363607015032511</v>
       </c>
       <c r="R6" t="n">
-        <v>2461</v>
+        <v>0.9033237093124847</v>
       </c>
       <c r="S6" t="n">
-        <v>4</v>
+        <v>0.9736842105263158</v>
       </c>
       <c r="T6" t="n">
+        <v>0.8409090909090909</v>
+      </c>
+      <c r="U6" t="n">
+        <v>2455</v>
+      </c>
+      <c r="V6" t="n">
+        <v>7</v>
+      </c>
+      <c r="W6" t="n">
         <v>1</v>
       </c>
-      <c r="U6" t="n">
-        <v>34</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0.9703017473220825</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0.9008556604385376</v>
-      </c>
       <c r="X6" t="n">
-        <v>0.9764554500579834</v>
+        <v>37</v>
       </c>
       <c r="Y6" t="n">
+        <v>0.9544999999999999</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.8867600000000001</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0.965</v>
+      </c>
+      <c r="AB6" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1659,75 +1999,84 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.856861591339111</v>
+        <v>2.820777343679271</v>
       </c>
       <c r="C7" t="n">
-        <v>12.95356273651123</v>
+        <v>12.94702117417342</v>
       </c>
       <c r="D7" t="n">
-        <v>12.95356273651123</v>
+        <v>12.90511742262838</v>
       </c>
       <c r="E7" t="n">
-        <v>12.95356273651123</v>
+        <v>12.98580278974723</v>
       </c>
       <c r="F7" t="n">
-        <v>0.09207551926374435</v>
+        <v>0.0945787473335622</v>
       </c>
       <c r="G7" t="n">
-        <v>0.09207551926374435</v>
+        <v>0.08283019320021789</v>
       </c>
       <c r="H7" t="n">
-        <v>0.09207551926374435</v>
+        <v>0.1081729615096668</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7026035189628601</v>
+        <v>0.7258313331048849</v>
       </c>
       <c r="J7" t="n">
-        <v>0.7026035189628601</v>
+        <v>0.7053390375734139</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7026035189628601</v>
+        <v>0.7487776044421424</v>
       </c>
       <c r="L7" t="n">
-        <v>0.6190255284309387</v>
+        <v>0.5995972402344912</v>
       </c>
       <c r="M7" t="n">
-        <v>0.6190255284309387</v>
+        <v>0.5442019313546903</v>
       </c>
       <c r="N7" t="n">
-        <v>0.6190255284309387</v>
+        <v>0.6537218440500082</v>
       </c>
       <c r="O7" t="n">
-        <v>0.8468314755371513</v>
+        <v>0.105047125873579</v>
       </c>
       <c r="P7" t="n">
-        <v>0.8795180722891566</v>
+        <v>0.09031064122943075</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.8455598455598455</v>
+        <v>0.1212936571031958</v>
       </c>
       <c r="R7" t="n">
-        <v>2211</v>
+        <v>0.8695127509638102</v>
       </c>
       <c r="S7" t="n">
-        <v>40</v>
+        <v>0.9152542372881356</v>
       </c>
       <c r="T7" t="n">
-        <v>30</v>
+        <v>0.8503937007874016</v>
       </c>
       <c r="U7" t="n">
-        <v>219</v>
+        <v>2226</v>
       </c>
       <c r="V7" t="n">
-        <v>0.8639162182807922</v>
+        <v>38</v>
       </c>
       <c r="W7" t="n">
-        <v>0.6288945078849792</v>
+        <v>20</v>
       </c>
       <c r="X7" t="n">
-        <v>0.9213899374008179</v>
+        <v>216</v>
       </c>
       <c r="Y7" t="n">
+        <v>0.8714999999999999</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.6677999999999999</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0.9266000000000001</v>
+      </c>
+      <c r="AB7" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1738,75 +2087,84 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.441611289978027</v>
+        <v>2.460613494406112</v>
       </c>
       <c r="C8" t="n">
-        <v>16.13397026062012</v>
+        <v>16.11422245069134</v>
       </c>
       <c r="D8" t="n">
-        <v>16.13397026062012</v>
+        <v>16.06959474573135</v>
       </c>
       <c r="E8" t="n">
-        <v>16.13397026062012</v>
+        <v>16.15639545615647</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1733374446630478</v>
+        <v>0.1657547039565893</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1733374446630478</v>
+        <v>0.1523722032298558</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1733374446630478</v>
+        <v>0.1812124664109969</v>
       </c>
       <c r="I8" t="n">
-        <v>2.481159526723786e-07</v>
+        <v>0.0004664724642728806</v>
       </c>
       <c r="J8" t="n">
-        <v>2.481159526723786e-07</v>
+        <v>4.911918071145661e-05</v>
       </c>
       <c r="K8" t="n">
-        <v>2.481159526723786e-07</v>
+        <v>0.001257983555216255</v>
       </c>
       <c r="L8" t="n">
-        <v>0.4753799140453339</v>
+        <v>0.4688225083160384</v>
       </c>
       <c r="M8" t="n">
-        <v>0.4753799140453339</v>
+        <v>0.4465290479576838</v>
       </c>
       <c r="N8" t="n">
-        <v>0.4753799140453339</v>
+        <v>0.4865683991115414</v>
       </c>
       <c r="O8" t="n">
-        <v>0.9971093359811521</v>
+        <v>0.1987618891000809</v>
       </c>
       <c r="P8" t="n">
+        <v>0.1797631382424711</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.2213180636352867</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.9970401771586715</v>
+      </c>
+      <c r="S8" t="n">
         <v>1</v>
       </c>
-      <c r="Q8" t="n">
-        <v>0.9951807228915662</v>
-      </c>
-      <c r="R8" t="n">
-        <v>2085</v>
-      </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
+        <v>0.9950372208436724</v>
+      </c>
+      <c r="U8" t="n">
+        <v>2097</v>
+      </c>
+      <c r="V8" t="n">
         <v>2</v>
       </c>
-      <c r="T8" t="n">
+      <c r="W8" t="n">
         <v>0</v>
       </c>
-      <c r="U8" t="n">
-        <v>413</v>
-      </c>
-      <c r="V8" t="n">
-        <v>0.9999998807907104</v>
-      </c>
-      <c r="W8" t="n">
-        <v>0.9999998807907104</v>
-      </c>
       <c r="X8" t="n">
-        <v>0.9999998807907104</v>
+        <v>401</v>
       </c>
       <c r="Y8" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB8" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1817,75 +2175,84 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.926028490066528</v>
+        <v>3.706092142790484</v>
       </c>
       <c r="C9" t="n">
-        <v>7.194806575775146</v>
+        <v>7.189457193415661</v>
       </c>
       <c r="D9" t="n">
-        <v>7.194806575775146</v>
+        <v>7.168334073955047</v>
       </c>
       <c r="E9" t="n">
-        <v>7.194806575775146</v>
+        <v>7.210659469287853</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02366244420409203</v>
+        <v>0.01020029171661144</v>
       </c>
       <c r="G9" t="n">
-        <v>0.02366244420409203</v>
+        <v>0.005897265310872962</v>
       </c>
       <c r="H9" t="n">
-        <v>0.02366244420409203</v>
+        <v>0.01526522430170675</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5380235910415649</v>
+        <v>0.5194858773447036</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5380235910415649</v>
+        <v>0.5006538765897894</v>
       </c>
       <c r="K9" t="n">
-        <v>0.5380235910415649</v>
+        <v>0.5366505686294555</v>
       </c>
       <c r="L9" t="n">
-        <v>3.483572721481323</v>
+        <v>0.4104453154206703</v>
       </c>
       <c r="M9" t="n">
-        <v>3.483572721481323</v>
+        <v>0.2961266557777721</v>
       </c>
       <c r="N9" t="n">
-        <v>3.483572721481323</v>
+        <v>0.5480921572713078</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.003743263765714322</v>
+        <v>0.0102009617696054</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>0.005932249577091742</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>0.01550190069323098</v>
       </c>
       <c r="R9" t="n">
-        <v>2455</v>
+        <v>0.8714594508585622</v>
       </c>
       <c r="S9" t="n">
-        <v>2</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="T9" t="n">
-        <v>43</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>2469</v>
       </c>
       <c r="V9" t="n">
-        <v>0.07034433633089066</v>
+        <v>3</v>
       </c>
       <c r="W9" t="n">
-        <v>0.0692678689956665</v>
+        <v>4</v>
       </c>
       <c r="X9" t="n">
-        <v>0.1757303029298782</v>
+        <v>24</v>
       </c>
       <c r="Y9" t="n">
+        <v>0.6850000000000001</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0.5242800000000001</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0.74912</v>
+      </c>
+      <c r="AB9" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1896,75 +2263,84 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4.359662055969238</v>
+        <v>4.341665515022483</v>
       </c>
       <c r="C10" t="n">
-        <v>5.326815605163574</v>
+        <v>5.33468568124798</v>
       </c>
       <c r="D10" t="n">
-        <v>5.326815605163574</v>
+        <v>5.319706065861732</v>
       </c>
       <c r="E10" t="n">
-        <v>5.326815605163574</v>
+        <v>5.347492325951338</v>
       </c>
       <c r="F10" t="n">
-        <v>0.373297244310379</v>
+        <v>0.3914118198340122</v>
       </c>
       <c r="G10" t="n">
-        <v>0.373297244310379</v>
+        <v>0.3705664963995696</v>
       </c>
       <c r="H10" t="n">
-        <v>0.373297244310379</v>
+        <v>0.4087058856405628</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0838344395160675</v>
+        <v>0.08353542977209527</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0838344395160675</v>
+        <v>0.07523268602758364</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0838344395160675</v>
+        <v>0.09153026863514424</v>
       </c>
       <c r="L10" t="n">
-        <v>0.3122648000717163</v>
+        <v>0.3060610510643892</v>
       </c>
       <c r="M10" t="n">
-        <v>0.3122648000717163</v>
+        <v>0.2968437687843908</v>
       </c>
       <c r="N10" t="n">
-        <v>0.3122648000717163</v>
+        <v>0.3150726422392233</v>
       </c>
       <c r="O10" t="n">
-        <v>0.9913434445727808</v>
+        <v>0.6421470399079152</v>
       </c>
       <c r="P10" t="n">
-        <v>0.9988839285714286</v>
+        <v>0.5887307301363743</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.9900442477876106</v>
+        <v>0.6912059232350666</v>
       </c>
       <c r="R10" t="n">
-        <v>1595</v>
+        <v>0.9932346972546198</v>
       </c>
       <c r="S10" t="n">
-        <v>9</v>
+        <v>0.9968684759916493</v>
       </c>
       <c r="T10" t="n">
+        <v>0.9947916666666666</v>
+      </c>
+      <c r="U10" t="n">
+        <v>1537</v>
+      </c>
+      <c r="V10" t="n">
+        <v>5</v>
+      </c>
+      <c r="W10" t="n">
+        <v>3</v>
+      </c>
+      <c r="X10" t="n">
+        <v>955</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.999</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0.997</v>
+      </c>
+      <c r="AA10" t="n">
         <v>1</v>
       </c>
-      <c r="U10" t="n">
-        <v>895</v>
-      </c>
-      <c r="V10" t="n">
-        <v>0.9992002248764038</v>
-      </c>
-      <c r="W10" t="n">
-        <v>0.9979904294013977</v>
-      </c>
-      <c r="X10" t="n">
-        <v>0.999485194683075</v>
-      </c>
-      <c r="Y10" t="n">
+      <c r="AB10" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1975,75 +2351,84 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3.186431884765625</v>
+        <v>3.225472119305814</v>
       </c>
       <c r="C11" t="n">
-        <v>9.840414047241211</v>
+        <v>9.852339237226829</v>
       </c>
       <c r="D11" t="n">
-        <v>9.840414047241211</v>
+        <v>9.824082008458316</v>
       </c>
       <c r="E11" t="n">
-        <v>9.840414047241211</v>
+        <v>9.884350406677033</v>
       </c>
       <c r="F11" t="n">
-        <v>0.08785878121852875</v>
+        <v>0.08448560331605469</v>
       </c>
       <c r="G11" t="n">
-        <v>0.08785878121852875</v>
+        <v>0.07309520044009686</v>
       </c>
       <c r="H11" t="n">
-        <v>0.08785878121852875</v>
+        <v>0.09676195628593512</v>
       </c>
       <c r="I11" t="n">
-        <v>0.006122462917119265</v>
+        <v>0.006639461118016384</v>
       </c>
       <c r="J11" t="n">
-        <v>0.006122462917119265</v>
+        <v>0.004579100021609141</v>
       </c>
       <c r="K11" t="n">
-        <v>0.006122462917119265</v>
+        <v>0.009203667677066311</v>
       </c>
       <c r="L11" t="n">
-        <v>0.3962530493736267</v>
+        <v>0.3956010195648135</v>
       </c>
       <c r="M11" t="n">
-        <v>0.3962530493736267</v>
+        <v>0.3677060567201618</v>
       </c>
       <c r="N11" t="n">
-        <v>0.3962530493736267</v>
+        <v>0.4207985087232566</v>
       </c>
       <c r="O11" t="n">
+        <v>0.09192504785077718</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.07885944972352504</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.1071279030234455</v>
+      </c>
+      <c r="R11" t="n">
         <v>1</v>
       </c>
-      <c r="P11" t="n">
+      <c r="S11" t="n">
         <v>1</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="T11" t="n">
         <v>1</v>
       </c>
-      <c r="R11" t="n">
-        <v>2288</v>
-      </c>
-      <c r="S11" t="n">
+      <c r="U11" t="n">
+        <v>2295</v>
+      </c>
+      <c r="V11" t="n">
         <v>0</v>
       </c>
-      <c r="T11" t="n">
+      <c r="W11" t="n">
         <v>0</v>
       </c>
-      <c r="U11" t="n">
-        <v>212</v>
-      </c>
-      <c r="V11" t="n">
-        <v>0.9994146227836609</v>
-      </c>
-      <c r="W11" t="n">
-        <v>0.998668909072876</v>
-      </c>
       <c r="X11" t="n">
-        <v>0.9996210336685181</v>
+        <v>205</v>
       </c>
       <c r="Y11" t="n">
+        <v>0.999</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0.9969999999999999</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB11" t="n">
         <v>9</v>
       </c>
     </row>
@@ -2054,75 +2439,84 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.973607301712036</v>
+        <v>2.995375448373186</v>
       </c>
       <c r="C12" t="n">
-        <v>11.95502662658691</v>
+        <v>11.96322958183414</v>
       </c>
       <c r="D12" t="n">
-        <v>11.95502662658691</v>
+        <v>11.92870514055968</v>
       </c>
       <c r="E12" t="n">
-        <v>11.95502662658691</v>
+        <v>11.99368550994363</v>
       </c>
       <c r="F12" t="n">
-        <v>0.05302276089787483</v>
+        <v>0.0533794672377056</v>
       </c>
       <c r="G12" t="n">
-        <v>0.05302276089787483</v>
+        <v>0.04369464973009872</v>
       </c>
       <c r="H12" t="n">
-        <v>0.05302276089787483</v>
+        <v>0.06487659669038243</v>
       </c>
       <c r="I12" t="n">
-        <v>0.7815248370170593</v>
+        <v>0.7945182412921981</v>
       </c>
       <c r="J12" t="n">
-        <v>0.7815248370170593</v>
+        <v>0.7693839250966474</v>
       </c>
       <c r="K12" t="n">
-        <v>0.7815248370170593</v>
+        <v>0.8190209699247484</v>
       </c>
       <c r="L12" t="n">
-        <v>0.5533568859100342</v>
+        <v>0.5551585792470073</v>
       </c>
       <c r="M12" t="n">
-        <v>0.5533568859100342</v>
+        <v>0.4795499899029492</v>
       </c>
       <c r="N12" t="n">
-        <v>0.5533568859100342</v>
+        <v>0.6384060213850387</v>
       </c>
       <c r="O12" t="n">
-        <v>0.7868520429585433</v>
+        <v>0.05658047681947021</v>
       </c>
       <c r="P12" t="n">
-        <v>0.8273381294964028</v>
+        <v>0.04569111141024397</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.7718120805369127</v>
+        <v>0.0693775785625913</v>
       </c>
       <c r="R12" t="n">
-        <v>2327</v>
+        <v>0.7935906365616388</v>
       </c>
       <c r="S12" t="n">
-        <v>34</v>
+        <v>0.8540145985401459</v>
       </c>
       <c r="T12" t="n">
-        <v>24</v>
+        <v>0.7597402597402597</v>
       </c>
       <c r="U12" t="n">
-        <v>115</v>
+        <v>2326</v>
       </c>
       <c r="V12" t="n">
-        <v>0.8027804493904114</v>
+        <v>37</v>
       </c>
       <c r="W12" t="n">
-        <v>0.4753356575965881</v>
+        <v>20</v>
       </c>
       <c r="X12" t="n">
-        <v>0.8996504545211792</v>
+        <v>117</v>
       </c>
       <c r="Y12" t="n">
+        <v>0.804</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.51184</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0.896</v>
+      </c>
+      <c r="AB12" t="n">
         <v>10</v>
       </c>
     </row>
@@ -2133,75 +2527,84 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.154835939407349</v>
+        <v>3.170628798538553</v>
       </c>
       <c r="C13" t="n">
-        <v>9.631141662597656</v>
+        <v>9.639543698313695</v>
       </c>
       <c r="D13" t="n">
-        <v>9.631141662597656</v>
+        <v>9.611562477102609</v>
       </c>
       <c r="E13" t="n">
-        <v>9.631141662597656</v>
+        <v>9.665630032700554</v>
       </c>
       <c r="F13" t="n">
-        <v>0.07902420312166214</v>
+        <v>0.08480423731309016</v>
       </c>
       <c r="G13" t="n">
-        <v>0.07902420312166214</v>
+        <v>0.07386499388506002</v>
       </c>
       <c r="H13" t="n">
-        <v>0.07902420312166214</v>
+        <v>0.0960858910530957</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1854678988456726</v>
+        <v>0.1937267553945467</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1854678988456726</v>
+        <v>0.1814808496724457</v>
       </c>
       <c r="K13" t="n">
-        <v>0.1854678988456726</v>
+        <v>0.2052193795159723</v>
       </c>
       <c r="L13" t="n">
-        <v>0.4235954880714417</v>
+        <v>0.3662738830980404</v>
       </c>
       <c r="M13" t="n">
-        <v>0.4235954880714417</v>
+        <v>0.3393094966662847</v>
       </c>
       <c r="N13" t="n">
-        <v>0.4235954880714417</v>
+        <v>0.3947897537012099</v>
       </c>
       <c r="O13" t="n">
-        <v>0.9287218132761675</v>
+        <v>0.09286683238074721</v>
       </c>
       <c r="P13" t="n">
-        <v>0.9583333333333334</v>
+        <v>0.07975618876184359</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.9108910891089109</v>
+        <v>0.1062998184553944</v>
       </c>
       <c r="R13" t="n">
-        <v>2290</v>
+        <v>0.943597182641281</v>
       </c>
       <c r="S13" t="n">
-        <v>18</v>
+        <v>0.957345971563981</v>
       </c>
       <c r="T13" t="n">
-        <v>8</v>
+        <v>0.9395348837209302</v>
       </c>
       <c r="U13" t="n">
-        <v>184</v>
+        <v>2276</v>
       </c>
       <c r="V13" t="n">
-        <v>0.9794950485229492</v>
+        <v>13</v>
       </c>
       <c r="W13" t="n">
-        <v>0.9295405149459839</v>
+        <v>9</v>
       </c>
       <c r="X13" t="n">
-        <v>0.9863492250442505</v>
+        <v>202</v>
       </c>
       <c r="Y13" t="n">
+        <v>0.979</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.9283999999999999</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="AB13" t="n">
         <v>11</v>
       </c>
     </row>
@@ -2212,75 +2615,84 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3.121087551116943</v>
+        <v>3.142391299649779</v>
       </c>
       <c r="C14" t="n">
-        <v>10.03303718566895</v>
+        <v>10.03569852759441</v>
       </c>
       <c r="D14" t="n">
-        <v>10.03303718566895</v>
+        <v>10.01061826186903</v>
       </c>
       <c r="E14" t="n">
-        <v>10.03303718566895</v>
+        <v>10.06206531456585</v>
       </c>
       <c r="F14" t="n">
-        <v>0.08428747951984406</v>
+        <v>0.09525387718336706</v>
       </c>
       <c r="G14" t="n">
-        <v>0.08428747951984406</v>
+        <v>0.08346382201397412</v>
       </c>
       <c r="H14" t="n">
-        <v>0.08428747951984406</v>
+        <v>0.1066966201665202</v>
       </c>
       <c r="I14" t="n">
-        <v>0.008974655531346798</v>
+        <v>0.01015939136549853</v>
       </c>
       <c r="J14" t="n">
-        <v>0.008974655531346798</v>
+        <v>0.007458203052389835</v>
       </c>
       <c r="K14" t="n">
-        <v>0.008974655531346798</v>
+        <v>0.01281235947068156</v>
       </c>
       <c r="L14" t="n">
-        <v>0.3652556836605072</v>
+        <v>0.360246998408932</v>
       </c>
       <c r="M14" t="n">
-        <v>0.3652556836605072</v>
+        <v>0.3415564031252638</v>
       </c>
       <c r="N14" t="n">
-        <v>0.3652556836605072</v>
+        <v>0.3817184203923227</v>
       </c>
       <c r="O14" t="n">
-        <v>0.9973407320146569</v>
+        <v>0.1050110262372095</v>
       </c>
       <c r="P14" t="n">
+        <v>0.09106441517159344</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.1194405408465576</v>
+      </c>
+      <c r="R14" t="n">
         <v>1</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0.9951219512195122</v>
-      </c>
-      <c r="R14" t="n">
-        <v>2295</v>
       </c>
       <c r="S14" t="n">
         <v>1</v>
       </c>
       <c r="T14" t="n">
+        <v>1</v>
+      </c>
+      <c r="U14" t="n">
+        <v>2267</v>
+      </c>
+      <c r="V14" t="n">
         <v>0</v>
       </c>
-      <c r="U14" t="n">
-        <v>204</v>
-      </c>
-      <c r="V14" t="n">
-        <v>0.9992063641548157</v>
-      </c>
       <c r="W14" t="n">
-        <v>0.9981458187103271</v>
+        <v>0</v>
       </c>
       <c r="X14" t="n">
-        <v>0.9994814395904541</v>
+        <v>233</v>
       </c>
       <c r="Y14" t="n">
+        <v>0.999</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0.997</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB14" t="n">
         <v>12</v>
       </c>
     </row>
@@ -2291,75 +2703,84 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4.105138778686523</v>
+        <v>4.137208684670553</v>
       </c>
       <c r="C15" t="n">
-        <v>5.945113658905029</v>
+        <v>5.947734231751868</v>
       </c>
       <c r="D15" t="n">
-        <v>5.945113658905029</v>
+        <v>5.930272223649119</v>
       </c>
       <c r="E15" t="n">
-        <v>5.945113658905029</v>
+        <v>5.963940386589615</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1038628146052361</v>
+        <v>0.09642714116542812</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1038628146052361</v>
+        <v>0.08595998786369696</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1038628146052361</v>
+        <v>0.1077907369339699</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1862469911575317</v>
+        <v>0.1895437997641797</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1862469911575317</v>
+        <v>0.1772588258055759</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1862469911575317</v>
+        <v>0.2013408244594097</v>
       </c>
       <c r="L15" t="n">
-        <v>0.2945449948310852</v>
+        <v>0.2868067900639515</v>
       </c>
       <c r="M15" t="n">
-        <v>0.2945449948310852</v>
+        <v>0.2679143789652279</v>
       </c>
       <c r="N15" t="n">
-        <v>0.2945449948310852</v>
+        <v>0.3090758418731739</v>
       </c>
       <c r="O15" t="n">
-        <v>0.9566674675666317</v>
+        <v>0.1071752170226099</v>
       </c>
       <c r="P15" t="n">
-        <v>0.9686274509803922</v>
+        <v>0.09404401918405748</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.9536679536679536</v>
+        <v>0.1208132908030957</v>
       </c>
       <c r="R15" t="n">
-        <v>2233</v>
+        <v>0.9795481656277086</v>
       </c>
       <c r="S15" t="n">
-        <v>12</v>
+        <v>0.987603305785124</v>
       </c>
       <c r="T15" t="n">
-        <v>8</v>
+        <v>0.9755102040816327</v>
       </c>
       <c r="U15" t="n">
-        <v>247</v>
+        <v>2252</v>
       </c>
       <c r="V15" t="n">
-        <v>0.9915199875831604</v>
+        <v>6</v>
       </c>
       <c r="W15" t="n">
-        <v>0.9758484959602356</v>
+        <v>3</v>
       </c>
       <c r="X15" t="n">
-        <v>0.994637131690979</v>
+        <v>239</v>
       </c>
       <c r="Y15" t="n">
+        <v>0.989</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0.9949999999999999</v>
+      </c>
+      <c r="AB15" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2370,75 +2791,84 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>5.820144653320312</v>
+        <v>5.88473809116669</v>
       </c>
       <c r="C16" t="n">
-        <v>3.031878709793091</v>
+        <v>3.027888286423714</v>
       </c>
       <c r="D16" t="n">
-        <v>3.031878709793091</v>
+        <v>3.019918136363977</v>
       </c>
       <c r="E16" t="n">
-        <v>3.031878709793091</v>
+        <v>3.03650264709537</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1038229390978813</v>
+        <v>0.0872624163775057</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1038229390978813</v>
+        <v>0.07619634851159757</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1038229390978813</v>
+        <v>0.09898511275115454</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2583747208118439</v>
+        <v>0.2767966375015812</v>
       </c>
       <c r="J16" t="n">
-        <v>0.2583747208118439</v>
+        <v>0.2642347862114395</v>
       </c>
       <c r="K16" t="n">
-        <v>0.2583747208118439</v>
+        <v>0.2903763093199611</v>
       </c>
       <c r="L16" t="n">
-        <v>0.3160667419433594</v>
+        <v>0.2953417896593574</v>
       </c>
       <c r="M16" t="n">
-        <v>0.3160667419433594</v>
+        <v>0.274387485007794</v>
       </c>
       <c r="N16" t="n">
-        <v>0.3160667419433594</v>
+        <v>0.3194380786617284</v>
       </c>
       <c r="O16" t="n">
-        <v>0.9679710744099679</v>
+        <v>0.09556660051866873</v>
       </c>
       <c r="P16" t="n">
-        <v>0.9731800766283525</v>
+        <v>0.08248110965965942</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.9694656488549618</v>
+        <v>0.1098595752348946</v>
       </c>
       <c r="R16" t="n">
-        <v>2231</v>
+        <v>0.9806306141685732</v>
       </c>
       <c r="S16" t="n">
-        <v>8</v>
+        <v>0.9867256637168141</v>
       </c>
       <c r="T16" t="n">
-        <v>7</v>
+        <v>0.9780701754385965</v>
       </c>
       <c r="U16" t="n">
-        <v>254</v>
+        <v>2269</v>
       </c>
       <c r="V16" t="n">
-        <v>0.9879155158996582</v>
+        <v>5</v>
       </c>
       <c r="W16" t="n">
-        <v>0.9623759388923645</v>
+        <v>3</v>
       </c>
       <c r="X16" t="n">
-        <v>0.9922677278518677</v>
+        <v>223</v>
       </c>
       <c r="Y16" t="n">
+        <v>0.985</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0.951</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0.993</v>
+      </c>
+      <c r="AB16" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2448,76 +2878,83 @@
           <t>seed15</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>2.099262237548828</v>
-      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
-        <v>19.60490417480469</v>
+        <v>19.5534935159926</v>
       </c>
       <c r="D17" t="n">
-        <v>19.60490417480469</v>
+        <v>19.49676170386515</v>
       </c>
       <c r="E17" t="n">
-        <v>19.60490417480469</v>
+        <v>19.60943952975702</v>
       </c>
       <c r="F17" t="n">
-        <v>2.55362682919458e-39</v>
+        <v>0.001554143868596999</v>
       </c>
       <c r="G17" t="n">
-        <v>2.55362682919458e-39</v>
+        <v>7.860107392213865e-06</v>
       </c>
       <c r="H17" t="n">
-        <v>2.55362682919458e-39</v>
+        <v>0.006028340086713864</v>
       </c>
       <c r="I17" t="n">
-        <v>0.9051593542098999</v>
+        <v>0.9381811838186331</v>
       </c>
       <c r="J17" t="n">
-        <v>0.9051593542098999</v>
+        <v>0.9152259560596872</v>
       </c>
       <c r="K17" t="n">
-        <v>0.9051593542098999</v>
+        <v>0.9617691055247519</v>
       </c>
       <c r="L17" t="n">
-        <v>0.004385115578770638</v>
+        <v>1.078968757426121</v>
       </c>
       <c r="M17" t="n">
-        <v>0.004385115578770638</v>
+        <v>0.07249672222266718</v>
       </c>
       <c r="N17" t="n">
-        <v>0.004385115578770638</v>
+        <v>2.822832924573759</v>
       </c>
       <c r="O17" t="n">
-        <v>0.02870602466483769</v>
+        <v>0.001459006685572768</v>
       </c>
       <c r="P17" t="n">
-        <v>1</v>
+        <v>7.860169265953495e-06</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.001623376623376623</v>
+        <v>0.006064905501311529</v>
       </c>
       <c r="R17" t="n">
-        <v>1268</v>
+        <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>1230</v>
+        <v>0</v>
       </c>
       <c r="T17" t="n">
         <v>0</v>
       </c>
       <c r="U17" t="n">
-        <v>2</v>
+        <v>2497</v>
       </c>
       <c r="V17" t="n">
-        <v>0.9999831914901733</v>
+        <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>0.9999764561653137</v>
+        <v>3</v>
       </c>
       <c r="X17" t="n">
-        <v>0.999989926815033</v>
+        <v>0</v>
       </c>
       <c r="Y17" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0.07284</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>0.11228</v>
+      </c>
+      <c r="AB17" t="n">
         <v>15</v>
       </c>
     </row>
@@ -2528,75 +2965,84 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3.603120565414429</v>
+        <v>3.613792346520083</v>
       </c>
       <c r="C18" t="n">
-        <v>7.919201850891113</v>
+        <v>7.93453673967796</v>
       </c>
       <c r="D18" t="n">
-        <v>7.919201850891113</v>
+        <v>7.914623340666387</v>
       </c>
       <c r="E18" t="n">
-        <v>7.919201850891113</v>
+        <v>7.953137699818162</v>
       </c>
       <c r="F18" t="n">
-        <v>0.07106241583824158</v>
+        <v>0.06591634814078702</v>
       </c>
       <c r="G18" t="n">
-        <v>0.07106241583824158</v>
+        <v>0.05701370651466432</v>
       </c>
       <c r="H18" t="n">
-        <v>0.07106241583824158</v>
+        <v>0.07654265809737852</v>
       </c>
       <c r="I18" t="n">
-        <v>0.4068015813827515</v>
+        <v>0.4042304089174305</v>
       </c>
       <c r="J18" t="n">
-        <v>0.4068015813827515</v>
+        <v>0.3874252446584953</v>
       </c>
       <c r="K18" t="n">
-        <v>0.4068015813827515</v>
+        <v>0.4201478162198955</v>
       </c>
       <c r="L18" t="n">
-        <v>0.4676582813262939</v>
+        <v>0.5248891185755938</v>
       </c>
       <c r="M18" t="n">
-        <v>0.4676582813262939</v>
+        <v>0.4697816465751792</v>
       </c>
       <c r="N18" t="n">
-        <v>0.4676582813262939</v>
+        <v>0.5790703851915633</v>
       </c>
       <c r="O18" t="n">
-        <v>0.8740188526182057</v>
+        <v>0.07103595557768196</v>
       </c>
       <c r="P18" t="n">
-        <v>0.9101123595505618</v>
+        <v>0.06046080890594997</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.08288707609378432</v>
       </c>
       <c r="R18" t="n">
-        <v>2295</v>
+        <v>0.8988725262020497</v>
       </c>
       <c r="S18" t="n">
-        <v>27</v>
+        <v>0.9349112426035503</v>
       </c>
       <c r="T18" t="n">
-        <v>16</v>
+        <v>0.8777777777777778</v>
       </c>
       <c r="U18" t="n">
-        <v>162</v>
+        <v>2309</v>
       </c>
       <c r="V18" t="n">
-        <v>0.9372369050979614</v>
+        <v>22</v>
       </c>
       <c r="W18" t="n">
-        <v>0.8232498168945312</v>
+        <v>11</v>
       </c>
       <c r="X18" t="n">
-        <v>0.9590663909912109</v>
+        <v>158</v>
       </c>
       <c r="Y18" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0.70788</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>0.95312</v>
+      </c>
+      <c r="AB18" t="n">
         <v>16</v>
       </c>
     </row>
@@ -2611,7 +3057,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2629,178 +3075,238 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>height</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Spot intensity</t>
+          <t>Number of on-target AOIs</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>width</t>
+          <t>F</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Spot width</t>
+          <t>Number of frames for on-target AOIs</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>snr</t>
+          <t>Nc</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Signal-to-noise ratio</t>
+          <t>Number of control off-target AOIs</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>background</t>
+          <t>Fc</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Image background</t>
+          <t>Number of frames for off-target AOIs</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
+          <t>P</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Average target-specific binding probability</t>
+          <t>Number of pixels along x- and y-axes of an AOI</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>lamda</t>
+          <t>height</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Non-specific binding rate</t>
+          <t>Spot intensity</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>proximity</t>
+          <t>width</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Proximity parameter</t>
+          <t>Spot width</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>z</t>
+          <t>snr</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>Signal-to-noise ratio</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>_ul</t>
+          <t>background</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>68% CI upper-limit</t>
+          <t>Image background</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>_ll</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>68% CI lower-limit</t>
+          <t>Average target-specific binding probability</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>lamda</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Matthews correlation coefficient</t>
+          <t>Non-specific binding rate</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>proximity</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>True positives</t>
+          <t>Proximity parameter</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>p(specific)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>False negatives</t>
+          <t>Probability of there being any target-specific spot in an AOI image</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>_ul</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>True negatives</t>
+          <t>95% CI upper-limit</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
+          <t>_ll</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>95% CI lower-limit</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>MCC</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Matthews correlation coefficient</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>True positives</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>False negatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>True negatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
           <t>FP</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>False positives</t>
         </is>

</xml_diff>